<commit_message>
Added code for a lockless linked list along with data from the three machines for key ranges 100, 100000 and 100000000.
</commit_message>
<xml_diff>
--- a/Data Structures/linked_list/Linked_List_Test_Data.xlsx
+++ b/Data Structures/linked_list/Linked_List_Test_Data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>64 Core Intel Xeon CPU E7-4820 @ 2.00GHz (A) Locked</t>
   </si>
@@ -93,14 +93,42 @@
     <t>16 Core Intel CPU @ 2.27 GHz (C ) CAS No Delay</t>
   </si>
   <si>
-    <t>Linked List Key Range 10000</t>
+    <t xml:space="preserve"> Locked Linked List Key Range 10000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lockless Linked List Key Range 100</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lockless Linked List Key Range 100000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lockless Linked List Key Range 100000000</t>
+  </si>
+  <si>
+    <t>Stoker</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
+  <si>
+    <t>Cube</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,19 +154,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:O101"/>
+  <dimension ref="A4:O110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:I9"/>
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,6 +486,7 @@
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="7" width="17.28515625" customWidth="1"/>
     <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -485,17 +522,17 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10">
@@ -527,28 +564,28 @@
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="7">
         <v>19352</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="7">
         <v>7691</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="7">
         <v>9197</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="7">
         <v>15179</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="7">
         <v>15582</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="7">
         <v>14771</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="7">
         <v>16412</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="7">
         <v>13288</v>
       </c>
     </row>
@@ -556,28 +593,28 @@
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="7">
         <v>19593</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="7">
         <v>18810</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="7">
         <v>22573</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="7">
         <v>2484151</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="7">
         <v>21938</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="7">
         <v>34588</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="7">
         <v>3361155</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="7">
         <v>5240420</v>
       </c>
     </row>
@@ -585,28 +622,28 @@
       <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="7">
         <v>19175</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="7">
         <v>22986</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="7">
         <v>44462</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="7">
         <v>111410</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="7">
         <v>210779</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="7">
         <v>361623</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="7">
         <v>436471</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="7">
         <v>410595</v>
       </c>
     </row>
@@ -614,28 +651,28 @@
       <c r="A14" t="s">
         <v>8</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="7">
         <v>18149</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="7">
         <v>3</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="7">
         <v>5</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="7">
         <v>9</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="7">
         <v>17</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="7">
         <v>33</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="7">
         <v>90</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="7">
         <v>129</v>
       </c>
     </row>
@@ -643,28 +680,28 @@
       <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="7">
         <v>22886</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="7">
         <v>11149</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="7">
         <v>21037</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="7">
         <v>15053</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="7">
         <v>8060</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="7">
         <v>8038</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="7">
         <v>8047</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="7">
         <v>6347</v>
       </c>
     </row>
@@ -672,28 +709,28 @@
       <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="7">
         <v>19312</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="7">
         <v>12582</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="7">
         <v>15298</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="7">
         <v>16114</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="7">
         <v>10882</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="7">
         <v>4506</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="7">
         <v>5291</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="7">
         <v>3019</v>
       </c>
     </row>
@@ -701,28 +738,28 @@
       <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="7">
         <v>18184</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="7">
         <v>11763</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="7">
         <v>11329</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="7">
         <v>10547</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="7">
         <v>11933</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="7">
         <v>12953</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="7">
         <v>14533</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="7">
         <v>8410</v>
       </c>
     </row>
@@ -730,28 +767,28 @@
       <c r="A18" t="s">
         <v>4</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="7">
         <v>17569</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="7">
         <v>11721</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="7">
         <v>8652</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="7">
         <v>11613</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="7">
         <v>7704</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="7">
         <v>6922</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="7">
         <v>6662</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="7">
         <v>6734</v>
       </c>
     </row>
@@ -759,28 +796,28 @@
       <c r="A19" t="s">
         <v>1</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="7">
         <v>33609</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="7">
         <v>47692</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="7">
         <v>49533</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="7">
         <v>40440</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="7">
         <v>47463</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="7">
         <v>47049</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="7">
         <v>47768</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="7">
         <v>47397</v>
       </c>
     </row>
@@ -788,28 +825,28 @@
       <c r="A20" t="s">
         <v>3</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="7">
         <v>33349</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="7">
         <v>5091146</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="7">
         <v>9784945</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="7">
         <v>33137</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="7">
         <v>43143</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="7">
         <v>57969</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="7">
         <v>43500</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="7">
         <v>75062</v>
       </c>
     </row>
@@ -817,28 +854,28 @@
       <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="7">
         <v>33478</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="7">
         <v>773845</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="7">
         <v>242735</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="7">
         <v>135142</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="7">
         <v>153953</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="7">
         <v>207157</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="7">
         <v>272692</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="7">
         <v>282835</v>
       </c>
     </row>
@@ -846,28 +883,28 @@
       <c r="A22" t="s">
         <v>7</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="7">
         <v>33606</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="7">
         <v>5</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="7">
         <v>6</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="7">
         <v>10</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="7">
         <v>18</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="7">
         <v>34</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="7">
         <v>65</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="7">
         <v>130</v>
       </c>
     </row>
@@ -875,28 +912,28 @@
       <c r="A23" t="s">
         <v>11</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="7">
         <v>33637</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="7">
         <v>21205</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="7">
         <v>21266</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="7">
         <v>20693</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="7">
         <v>21153</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="7">
         <v>21079</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="7">
         <v>20951</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="7">
         <v>20969</v>
       </c>
     </row>
@@ -904,28 +941,28 @@
       <c r="A24" t="s">
         <v>10</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="7">
         <v>33572</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="7">
         <v>25760</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="7">
         <v>53595</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="7">
         <v>57890</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="7">
         <v>35390</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="7">
         <v>32984</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="7">
         <v>44559</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="7">
         <v>35642</v>
       </c>
     </row>
@@ -933,28 +970,28 @@
       <c r="A25" t="s">
         <v>13</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="7">
         <v>33083</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="7">
         <v>23127</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="7">
         <v>21157</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="7">
         <v>17110</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="7">
         <v>17610</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="7">
         <v>16909</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="7">
         <v>16949</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="7">
         <v>21946</v>
       </c>
     </row>
@@ -962,28 +999,28 @@
       <c r="A26" t="s">
         <v>5</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="7">
         <v>33291</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="7">
         <v>21129</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="7">
         <v>21445</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="7">
         <v>21032</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="7">
         <v>21285</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="7">
         <v>21330</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="7">
         <v>21399</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="7">
         <v>21365</v>
       </c>
     </row>
@@ -991,28 +1028,28 @@
       <c r="A27" t="s">
         <v>14</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="7">
         <v>21222</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="7">
         <v>14819</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="7">
         <v>17862</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="7">
         <v>24680</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="7">
         <v>18891</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="7">
         <v>19095</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="7">
         <v>24403</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="7">
         <v>23015</v>
       </c>
     </row>
@@ -1020,28 +1057,28 @@
       <c r="A28" t="s">
         <v>15</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="7">
         <v>21006</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="7">
         <v>24590</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="7">
         <v>30433</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="7">
         <v>5507364</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="7">
         <v>6599426</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="7">
         <v>5532070</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="7">
         <v>5482486</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="7">
         <v>4436050</v>
       </c>
     </row>
@@ -1049,28 +1086,28 @@
       <c r="A29" t="s">
         <v>23</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="7">
         <v>20421</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="7">
         <v>24451</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="7">
         <v>66505</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="7">
         <v>138300</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="7">
         <v>126200</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="7">
         <v>264191</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="7">
         <v>164026</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="7">
         <v>162107</v>
       </c>
     </row>
@@ -1078,28 +1115,28 @@
       <c r="A30" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="8">
         <v>20943</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="8">
         <v>3</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="8">
         <v>5</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="8">
         <v>9</v>
       </c>
-      <c r="F30" s="4">
+      <c r="F30" s="8">
         <v>17</v>
       </c>
-      <c r="G30" s="4">
+      <c r="G30" s="8">
         <v>33</v>
       </c>
-      <c r="H30" s="4">
+      <c r="H30" s="8">
         <v>65</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="8">
         <v>129</v>
       </c>
     </row>
@@ -1107,28 +1144,28 @@
       <c r="A31" t="s">
         <v>17</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="7">
         <v>21302</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="7">
         <v>13890</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="7">
         <v>9375</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="7">
         <v>9131</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="7">
         <v>9104</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="7">
         <v>9142</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="7">
         <v>9108</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="7">
         <v>8986</v>
       </c>
     </row>
@@ -1136,239 +1173,595 @@
       <c r="A32" t="s">
         <v>18</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="7">
         <v>25344</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="7">
         <v>12883</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="7">
         <v>22546</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="7">
         <v>25361</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="7">
         <v>21629</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="7">
         <v>10489</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="7">
         <v>6302</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="7">
         <v>3007</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>19</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="7">
         <v>21042</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="7">
         <v>14108</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="7">
         <v>17173</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="7">
         <v>20160</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="7">
         <v>14047</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="7">
         <v>4095</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="7">
         <v>2912</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="7">
         <v>2201</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>20</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="7">
         <v>21409</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="7">
         <v>13265</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="7">
         <v>9085</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="7">
         <v>8949</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="7">
         <v>9022</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="7">
         <v>12421</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="7">
         <v>15532</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="7">
         <v>15632</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L41" s="1"/>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-      <c r="L43" s="1"/>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <v>4</v>
+      </c>
+      <c r="E39">
+        <v>8</v>
+      </c>
+      <c r="F39">
+        <v>16</v>
+      </c>
+      <c r="G39">
+        <v>32</v>
+      </c>
+      <c r="H39">
+        <v>64</v>
+      </c>
+      <c r="I39">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="8">
+        <v>1260361</v>
+      </c>
+      <c r="C40" s="8">
+        <v>3223245</v>
+      </c>
+      <c r="D40" s="8">
+        <v>3831773</v>
+      </c>
+      <c r="E40" s="8">
+        <v>2018335</v>
+      </c>
+      <c r="F40" s="8">
+        <v>1117124</v>
+      </c>
+      <c r="G40" s="8">
+        <v>973184</v>
+      </c>
+      <c r="H40" s="8">
+        <v>957302</v>
+      </c>
+      <c r="I40" s="8">
+        <v>872011</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="8">
+        <v>3088997</v>
+      </c>
+      <c r="C41" s="8">
+        <v>6476714</v>
+      </c>
+      <c r="D41" s="8">
+        <v>10930666</v>
+      </c>
+      <c r="E41" s="8">
+        <v>14064264</v>
+      </c>
+      <c r="F41" s="8">
+        <v>16707949</v>
+      </c>
+      <c r="G41" s="8">
+        <v>16452599</v>
+      </c>
+      <c r="H41" s="8">
+        <v>16119640</v>
+      </c>
+      <c r="I41" s="8">
+        <v>16283874</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="8">
+        <v>1564789</v>
+      </c>
+      <c r="C42" s="8">
+        <v>6644170</v>
+      </c>
+      <c r="D42" s="8">
+        <v>10082413</v>
+      </c>
+      <c r="E42" s="8">
+        <v>1485215</v>
+      </c>
+      <c r="F42" s="8">
+        <v>4991497</v>
+      </c>
+      <c r="G42" s="8">
+        <v>9434910</v>
+      </c>
+      <c r="H42" s="8">
+        <v>4795728</v>
+      </c>
+      <c r="I42" s="8">
+        <v>1563694</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="5"/>
       <c r="B44" s="1"/>
-      <c r="E44" s="2"/>
-      <c r="L44" s="1"/>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-      <c r="E45" s="2"/>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="5"/>
       <c r="L45" s="1"/>
-      <c r="O45" s="2"/>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-      <c r="L46" s="1"/>
-      <c r="O46" s="2"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="L47" s="1"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-    </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
-      <c r="E49" s="2"/>
-      <c r="L49" s="1"/>
-    </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L50" s="1"/>
-      <c r="O50" s="2"/>
-    </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>8</v>
+      </c>
+      <c r="F47">
+        <v>16</v>
+      </c>
+      <c r="G47">
+        <v>32</v>
+      </c>
+      <c r="H47">
+        <v>64</v>
+      </c>
+      <c r="I47">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48" s="8">
+        <v>13038</v>
+      </c>
+      <c r="C48" s="8">
+        <v>7707</v>
+      </c>
+      <c r="D48" s="8">
+        <v>11241</v>
+      </c>
+      <c r="E48" s="8">
+        <v>14850</v>
+      </c>
+      <c r="F48" s="8">
+        <v>19893</v>
+      </c>
+      <c r="G48" s="8">
+        <v>28269</v>
+      </c>
+      <c r="H48" s="8">
+        <v>36159</v>
+      </c>
+      <c r="I48" s="8">
+        <v>41713</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49" s="8">
+        <v>22102</v>
+      </c>
+      <c r="C49" s="8">
+        <v>19411</v>
+      </c>
+      <c r="D49" s="8">
+        <v>71947</v>
+      </c>
+      <c r="E49" s="8">
+        <v>390928</v>
+      </c>
+      <c r="F49" s="8">
+        <v>204303</v>
+      </c>
+      <c r="G49" s="8">
+        <v>441122</v>
+      </c>
+      <c r="H49" s="8">
+        <v>86648</v>
+      </c>
+      <c r="I49" s="8">
+        <v>393695</v>
+      </c>
+      <c r="L49" s="6"/>
+    </row>
+    <row r="50" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" s="8">
+        <v>15726</v>
+      </c>
+      <c r="C50" s="8">
+        <v>8789</v>
+      </c>
+      <c r="D50" s="8">
+        <v>15088</v>
+      </c>
+      <c r="E50" s="8">
+        <v>21429</v>
+      </c>
+      <c r="F50" s="8">
+        <v>26954</v>
+      </c>
+      <c r="G50" s="8">
+        <v>23518</v>
+      </c>
+      <c r="H50" s="8">
+        <v>21168</v>
+      </c>
+      <c r="I50" s="8">
+        <v>19748</v>
+      </c>
+      <c r="L50" s="6"/>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A51" s="5"/>
+      <c r="B51" s="1"/>
+      <c r="E51" s="2"/>
+      <c r="L51" s="1"/>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="1"/>
+      <c r="E52" s="2"/>
+      <c r="L52" s="1"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A53" s="5"/>
       <c r="B53" s="1"/>
-    </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
+      <c r="E53" s="2"/>
+      <c r="L53" s="1"/>
+      <c r="O53" s="2"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
       <c r="L54" s="1"/>
-    </row>
-    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-      <c r="L55" s="1"/>
-    </row>
-    <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
-      <c r="L56" s="1"/>
-    </row>
-    <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-      <c r="E57" s="2"/>
-      <c r="L57" s="1"/>
-    </row>
-    <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="E58" s="2"/>
-      <c r="L58" s="1"/>
-      <c r="O58" s="2"/>
-    </row>
-    <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
+      <c r="O54" s="2"/>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>4</v>
+      </c>
+      <c r="E55">
+        <v>8</v>
+      </c>
+      <c r="F55">
+        <v>16</v>
+      </c>
+      <c r="G55">
+        <v>32</v>
+      </c>
+      <c r="H55">
+        <v>64</v>
+      </c>
+      <c r="I55">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" s="8">
+        <v>12477</v>
+      </c>
+      <c r="C56" s="8">
+        <v>5590</v>
+      </c>
+      <c r="D56" s="8">
+        <v>8479</v>
+      </c>
+      <c r="E56" s="8">
+        <v>11799</v>
+      </c>
+      <c r="F56" s="8">
+        <v>16135</v>
+      </c>
+      <c r="G56" s="8">
+        <v>20660</v>
+      </c>
+      <c r="H56" s="8">
+        <v>23485</v>
+      </c>
+      <c r="I56" s="8">
+        <v>24492</v>
+      </c>
+      <c r="L56" s="6"/>
+    </row>
+    <row r="57" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" s="8">
+        <v>21346</v>
+      </c>
+      <c r="C57" s="8">
+        <v>19221</v>
+      </c>
+      <c r="D57" s="8">
+        <v>50195</v>
+      </c>
+      <c r="E57" s="8">
+        <v>90360</v>
+      </c>
+      <c r="F57" s="8">
+        <v>125158</v>
+      </c>
+      <c r="G57" s="8">
+        <v>57110</v>
+      </c>
+      <c r="H57" s="8">
+        <v>40420</v>
+      </c>
+      <c r="I57" s="8">
+        <v>34840</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" s="8">
+        <v>15387</v>
+      </c>
+      <c r="C58" s="8">
+        <v>7672</v>
+      </c>
+      <c r="D58" s="8">
+        <v>12221</v>
+      </c>
+      <c r="E58" s="8">
+        <v>17355</v>
+      </c>
+      <c r="F58" s="8">
+        <v>19129</v>
+      </c>
+      <c r="G58" s="8">
+        <v>15638</v>
+      </c>
+      <c r="H58" s="8">
+        <v>13232</v>
+      </c>
+      <c r="I58" s="8">
+        <v>11593</v>
+      </c>
+      <c r="L58" s="6"/>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="5"/>
       <c r="L59" s="1"/>
       <c r="O59" s="2"/>
     </row>
-    <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="L60" s="1"/>
-    </row>
-    <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="1"/>
-    </row>
-    <row r="62" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="5"/>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
       <c r="B62" s="1"/>
-      <c r="E62" s="2"/>
-      <c r="L62" s="1"/>
-    </row>
-    <row r="63" spans="2:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A63" s="5"/>
+      <c r="B63" s="1"/>
       <c r="L63" s="1"/>
-      <c r="O63" s="2"/>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B64" s="1"/>
+      <c r="L64" s="1"/>
+    </row>
+    <row r="65" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B65" s="1"/>
+      <c r="L65" s="1"/>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B66" s="1"/>
+      <c r="E66" s="2"/>
+      <c r="L66" s="1"/>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B67" s="1"/>
+      <c r="E67" s="2"/>
+      <c r="L67" s="1"/>
+      <c r="O67" s="2"/>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B68" s="1"/>
       <c r="L68" s="1"/>
+      <c r="O68" s="2"/>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="1"/>
       <c r="L69" s="1"/>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
-      <c r="E70" s="2"/>
-      <c r="L70" s="1"/>
-      <c r="O70" s="2"/>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="E71" s="2"/>
       <c r="L71" s="1"/>
-      <c r="O71" s="2"/>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="1"/>
       <c r="L72" s="1"/>
-    </row>
-    <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="1"/>
-      <c r="L74" s="1"/>
+      <c r="O72" s="2"/>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B75" s="1"/>
-      <c r="E75" s="2"/>
-      <c r="L75" s="1"/>
-      <c r="O75" s="2"/>
+    </row>
+    <row r="76" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B76" s="1"/>
+    </row>
+    <row r="77" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B77" s="1"/>
+      <c r="L77" s="1"/>
+    </row>
+    <row r="78" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B78" s="1"/>
+      <c r="L78" s="1"/>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B79" s="1"/>
+      <c r="E79" s="2"/>
       <c r="L79" s="1"/>
+      <c r="O79" s="2"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="1"/>
+      <c r="E80" s="2"/>
+      <c r="L80" s="1"/>
+      <c r="O80" s="2"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="L81" s="1"/>
     </row>
-    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B82" s="1"/>
-      <c r="L82" s="1"/>
-    </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
-      <c r="E83" s="2"/>
       <c r="L83" s="1"/>
-      <c r="O83" s="2"/>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
@@ -1376,33 +1769,40 @@
       <c r="L84" s="1"/>
       <c r="O84" s="2"/>
     </row>
-    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B85" s="1"/>
-      <c r="L85" s="1"/>
-    </row>
-    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B87" s="1"/>
-      <c r="L87" s="1"/>
-    </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
-      <c r="E88" s="2"/>
       <c r="L88" s="1"/>
-      <c r="O88" s="2"/>
+    </row>
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B89" s="1"/>
+    </row>
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B90" s="1"/>
+      <c r="L90" s="1"/>
+    </row>
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B91" s="1"/>
+      <c r="L91" s="1"/>
+    </row>
+    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B92" s="1"/>
+      <c r="E92" s="2"/>
+      <c r="L92" s="1"/>
+      <c r="O92" s="2"/>
+    </row>
+    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B93" s="1"/>
+      <c r="E93" s="2"/>
+      <c r="L93" s="1"/>
+      <c r="O93" s="2"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B94" s="1"/>
       <c r="L94" s="1"/>
     </row>
-    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B95" s="1"/>
-      <c r="L95" s="1"/>
-    </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B96" s="1"/>
-      <c r="E96" s="2"/>
       <c r="L96" s="1"/>
-      <c r="O96" s="2"/>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
@@ -1410,23 +1810,46 @@
       <c r="L97" s="1"/>
       <c r="O97" s="2"/>
     </row>
-    <row r="98" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B98" s="1"/>
-      <c r="L98" s="1"/>
-    </row>
-    <row r="100" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B100" s="1"/>
-      <c r="L100" s="1"/>
-    </row>
-    <row r="101" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B101" s="1"/>
-      <c r="E101" s="2"/>
-      <c r="L101" s="1"/>
-      <c r="O101" s="2"/>
+    <row r="103" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B103" s="1"/>
+      <c r="L103" s="1"/>
+    </row>
+    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B104" s="1"/>
+      <c r="L104" s="1"/>
+    </row>
+    <row r="105" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B105" s="1"/>
+      <c r="E105" s="2"/>
+      <c r="L105" s="1"/>
+      <c r="O105" s="2"/>
+    </row>
+    <row r="106" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B106" s="1"/>
+      <c r="E106" s="2"/>
+      <c r="L106" s="1"/>
+      <c r="O106" s="2"/>
+    </row>
+    <row r="107" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B107" s="1"/>
+      <c r="L107" s="1"/>
+    </row>
+    <row r="109" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B109" s="1"/>
+      <c r="L109" s="1"/>
+    </row>
+    <row r="110" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B110" s="1"/>
+      <c r="E110" s="2"/>
+      <c r="L110" s="1"/>
+      <c r="O110" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A9:I9"/>
+    <mergeCell ref="A38:I38"/>
+    <mergeCell ref="A46:I46"/>
+    <mergeCell ref="A54:I54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>